<commit_message>
11.03.21 внес 55 000
</commit_message>
<xml_diff>
--- a/tovar.xlsx
+++ b/tovar.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandon\Desktop\tovar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520F51EA-12E0-4C0D-A4DE-B36F9FF69CC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C1CF48-F400-42A1-9D2A-B3D808E608BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15660" xr2:uid="{BCDC4CE2-D9AE-46C6-8E0E-240183A36DBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>EZ-HAC-B2A41P-0280B-DIP Видеокамера HDCVI купольная, 1/2.7" 4Мп</t>
   </si>
@@ -317,7 +318,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -408,6 +409,24 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -728,12 +747,12 @@
   <dimension ref="A1:AQ74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="31" customWidth="1"/>
     <col min="2" max="2" width="73.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="4" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" style="4" customWidth="1"/>
@@ -763,7 +782,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="32">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -783,11 +802,11 @@
         <v>60</v>
       </c>
       <c r="J2" s="23">
-        <v>645000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="32">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -808,11 +827,11 @@
       </c>
       <c r="J3" s="25">
         <f>J2-J1</f>
-        <v>37642</v>
+        <v>92642</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="32">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -830,7 +849,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="32">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -848,7 +867,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="32">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -866,7 +885,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="32">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -884,7 +903,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="32">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -902,7 +921,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="32">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -920,7 +939,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="32">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -938,7 +957,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="32">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -956,7 +975,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="32">
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -974,7 +993,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="32">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -992,7 +1011,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="32">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1010,7 +1029,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="32">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1028,7 +1047,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="32">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1046,7 +1065,7 @@
       </c>
     </row>
     <row r="17" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="32">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1064,7 +1083,7 @@
       </c>
     </row>
     <row r="18" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="32">
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -1082,7 +1101,7 @@
       </c>
     </row>
     <row r="19" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="33"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="9"/>
@@ -1096,7 +1115,7 @@
       </c>
     </row>
     <row r="20" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+      <c r="A20" s="34">
         <v>18</v>
       </c>
       <c r="B20" s="11" t="s">
@@ -1120,7 +1139,7 @@
       <c r="K20" s="14"/>
     </row>
     <row r="21" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
+      <c r="A21" s="34">
         <v>19</v>
       </c>
       <c r="B21" s="11" t="s">
@@ -1176,7 +1195,7 @@
       <c r="AQ21" s="15"/>
     </row>
     <row r="22" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
+      <c r="A22" s="34">
         <v>20</v>
       </c>
       <c r="B22" s="11" t="s">
@@ -1232,7 +1251,7 @@
       <c r="AQ22" s="15"/>
     </row>
     <row r="23" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
+      <c r="A23" s="34">
         <v>21</v>
       </c>
       <c r="B23" s="11" t="s">
@@ -1288,7 +1307,7 @@
       <c r="AQ23" s="15"/>
     </row>
     <row r="24" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+      <c r="A24" s="34">
         <v>22</v>
       </c>
       <c r="B24" s="11" t="s">
@@ -1344,7 +1363,7 @@
       <c r="AQ24" s="15"/>
     </row>
     <row r="25" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
+      <c r="A25" s="34">
         <v>23</v>
       </c>
       <c r="B25" s="11" t="s">
@@ -1400,7 +1419,7 @@
       <c r="AQ25" s="15"/>
     </row>
     <row r="26" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
+      <c r="A26" s="34">
         <v>24</v>
       </c>
       <c r="B26" s="11" t="s">
@@ -1456,7 +1475,7 @@
       <c r="AQ26" s="15"/>
     </row>
     <row r="27" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
+      <c r="A27" s="34">
         <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
@@ -1512,7 +1531,7 @@
       <c r="AQ27" s="15"/>
     </row>
     <row r="28" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+      <c r="A28" s="34">
         <v>26</v>
       </c>
       <c r="B28" s="11" t="s">
@@ -1568,7 +1587,7 @@
       <c r="AQ28" s="15"/>
     </row>
     <row r="29" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
+      <c r="A29" s="34">
         <v>27</v>
       </c>
       <c r="B29" s="11" t="s">
@@ -1624,7 +1643,7 @@
       <c r="AQ29" s="15"/>
     </row>
     <row r="30" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
+      <c r="A30" s="34">
         <v>28</v>
       </c>
       <c r="B30" s="11" t="s">
@@ -1680,7 +1699,7 @@
       <c r="AQ30" s="15"/>
     </row>
     <row r="31" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
+      <c r="A31" s="34">
         <v>29</v>
       </c>
       <c r="B31" s="11" t="s">
@@ -1736,7 +1755,7 @@
       <c r="AQ31" s="15"/>
     </row>
     <row r="32" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
+      <c r="A32" s="34">
         <v>30</v>
       </c>
       <c r="B32" s="11" t="s">
@@ -1792,7 +1811,7 @@
       <c r="AQ32" s="15"/>
     </row>
     <row r="33" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
+      <c r="A33" s="34">
         <v>31</v>
       </c>
       <c r="B33" s="11" t="s">
@@ -1848,7 +1867,7 @@
       <c r="AQ33" s="15"/>
     </row>
     <row r="34" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10">
+      <c r="A34" s="34">
         <v>32</v>
       </c>
       <c r="B34" s="11" t="s">
@@ -1904,7 +1923,7 @@
       <c r="AQ34" s="15"/>
     </row>
     <row r="35" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10">
+      <c r="A35" s="34">
         <v>33</v>
       </c>
       <c r="B35" s="11" t="s">
@@ -1960,7 +1979,7 @@
       <c r="AQ35" s="15"/>
     </row>
     <row r="36" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10">
+      <c r="A36" s="34">
         <v>34</v>
       </c>
       <c r="B36" s="11" t="s">
@@ -2016,7 +2035,7 @@
       <c r="AQ36" s="15"/>
     </row>
     <row r="37" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="10">
+      <c r="A37" s="34">
         <v>35</v>
       </c>
       <c r="B37" s="11" t="s">
@@ -2120,7 +2139,7 @@
       <c r="AQ38" s="15"/>
     </row>
     <row r="39" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="17">
+      <c r="A39" s="35">
         <v>36</v>
       </c>
       <c r="B39" s="17" t="s">
@@ -2147,7 +2166,7 @@
       </c>
     </row>
     <row r="41" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="20">
+      <c r="A41" s="36">
         <v>37</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -2165,7 +2184,7 @@
       </c>
     </row>
     <row r="42" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="20">
+      <c r="A42" s="36">
         <v>38</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -2183,7 +2202,7 @@
       </c>
     </row>
     <row r="43" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="20">
+      <c r="A43" s="36">
         <v>39</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -2201,7 +2220,7 @@
       </c>
     </row>
     <row r="44" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="20">
+      <c r="A44" s="36">
         <v>40</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -2219,7 +2238,7 @@
       </c>
     </row>
     <row r="45" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="20">
+      <c r="A45" s="36">
         <v>41</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -2237,7 +2256,7 @@
       </c>
     </row>
     <row r="46" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="20">
+      <c r="A46" s="36">
         <v>42</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -2255,7 +2274,7 @@
       </c>
     </row>
     <row r="47" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="20">
+      <c r="A47" s="36">
         <v>43</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -2273,7 +2292,7 @@
       </c>
     </row>
     <row r="48" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="20">
+      <c r="A48" s="36">
         <v>44</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -2291,7 +2310,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="20">
+      <c r="A49" s="36">
         <v>45</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2309,7 +2328,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="20">
+      <c r="A50" s="36">
         <v>46</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2327,7 +2346,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="20">
+      <c r="A51" s="36">
         <v>47</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -2345,7 +2364,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="20">
+      <c r="A52" s="36">
         <v>48</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -2363,7 +2382,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="20">
+      <c r="A53" s="36">
         <v>49</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -2381,7 +2400,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="20">
+      <c r="A54" s="36">
         <v>50</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -2399,7 +2418,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="20">
+      <c r="A55" s="36">
         <v>51</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -2417,7 +2436,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="20">
+      <c r="A56" s="36">
         <v>52</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -2435,7 +2454,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="20">
+      <c r="A57" s="36">
         <v>53</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -2453,7 +2472,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="20">
+      <c r="A58" s="36">
         <v>54</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -2471,7 +2490,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="20">
+      <c r="A59" s="36">
         <v>55</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -2489,7 +2508,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="20">
+      <c r="A60" s="36">
         <v>56</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -2507,7 +2526,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="20">
+      <c r="A61" s="36">
         <v>57</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -2525,7 +2544,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="20">
+      <c r="A62" s="36">
         <v>58</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -2543,62 +2562,62 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
+      <c r="A63" s="31">
         <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="4">
+      <c r="A64" s="31">
         <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4">
+      <c r="A65" s="31">
         <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="4">
+      <c r="A66" s="31">
         <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4">
+      <c r="A67" s="31">
         <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="4">
+      <c r="A68" s="31">
         <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="4">
+      <c r="A69" s="31">
         <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="4">
+      <c r="A70" s="31">
         <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
+      <c r="A71" s="31">
         <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="4">
+      <c r="A72" s="31">
         <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="4">
+      <c r="A73" s="31">
         <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="4">
+      <c r="A74" s="31">
         <v>70</v>
       </c>
     </row>
@@ -2606,4 +2625,81 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50932C3E-E83F-4084-ACF3-705CC8D731D6}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="32">
+        <v>16</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="5">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7">
+        <v>4245</v>
+      </c>
+      <c r="E1" s="5">
+        <f t="shared" ref="E1:E3" si="0">C1*D1</f>
+        <v>4245</v>
+      </c>
+      <c r="H1">
+        <f>SUM(E:E)/5*6</f>
+        <v>15006</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="32">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1295</v>
+      </c>
+      <c r="E2" s="5">
+        <f t="shared" si="0"/>
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="32">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5">
+        <v>7</v>
+      </c>
+      <c r="D3" s="5">
+        <v>995</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" si="0"/>
+        <v>6965</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>